<commit_message>
final version of first milestone
</commit_message>
<xml_diff>
--- a/project1/data statistics.xlsx
+++ b/project1/data statistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jj\git\rpi\project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7904CE7-7BD1-43C2-B289-3E6D0F7C113D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B04C42-6470-44D7-AC59-C8DB5877C0A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" firstSheet="4" activeTab="6" xr2:uid="{DD7AB8B6-2DA4-4BE4-BABD-58FB573693DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" firstSheet="4" activeTab="5" xr2:uid="{DD7AB8B6-2DA4-4BE4-BABD-58FB573693DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Top level stats" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Overdue 60-89 days distribution" sheetId="5" r:id="rId5"/>
     <sheet name="Overdue 90+ days distribution" sheetId="6" r:id="rId6"/>
     <sheet name="Missing revenues" sheetId="7" r:id="rId7"/>
+    <sheet name="Credit rating correlation" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Type</t>
   </si>
@@ -135,13 +136,28 @@
   </si>
   <si>
     <t>~5.1</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Revenue corr.</t>
+  </si>
+  <si>
+    <t>Debt ratio corr.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="173" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +171,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -198,11 +220,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,10 +768,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721F8CC0-9864-4AC5-B89E-2DC9B4E9829C}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,6 +998,18 @@
       </c>
       <c r="C20">
         <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f>SUM(C2:C20)</f>
+        <v>45063</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <f>C2/C22</f>
+        <v>0.19179814925770589</v>
       </c>
     </row>
   </sheetData>
@@ -1080,7 +1118,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,8 +1395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7C4686-D246-447F-9675-AF8B4366D6B0}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,7 +1574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD07AC3A-2EF0-4A7D-ABD8-771D16B4D1DD}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1620,4 +1658,173 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6E19B4-A3F2-4989-BBFF-58461D100BC8}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>5799.0640000000003</v>
+      </c>
+      <c r="C2">
+        <v>418.714</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="3">
+        <f>CORREL(A2:A8,B2:B8)</f>
+        <v>0.95390986606408301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>6893.4979999999996</v>
+      </c>
+      <c r="C3">
+        <v>174.69800000000001</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="3">
+        <f>CORREL(A2:A8,C2:C8)</f>
+        <v>-0.6937099432163979</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>7198.6459999999997</v>
+      </c>
+      <c r="C4">
+        <v>263.03100000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>7490.268</v>
+      </c>
+      <c r="C5">
+        <v>227.625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>8302.8709999999992</v>
+      </c>
+      <c r="C6">
+        <v>181.32400000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>8587.1630000000005</v>
+      </c>
+      <c r="C7">
+        <v>172.709</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>8446.1540000000005</v>
+      </c>
+      <c r="C8">
+        <v>179.23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>8536.2309999999998</v>
+      </c>
+      <c r="C9">
+        <v>300.82799999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>4910</v>
+      </c>
+      <c r="C10">
+        <v>0.20599999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>2789</v>
+      </c>
+      <c r="C11">
+        <v>0.64400000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>7500</v>
+      </c>
+      <c r="C12">
+        <v>0.13400000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>